<commit_message>
- Se agregan fixtures para las pruebas. - Se codifica UI de la ventana principal. - Se conecta los servicios con el ViewModel y View.
</commit_message>
<xml_diff>
--- a/Tests/Fixtures/Excel/Empleado.xlsx
+++ b/Tests/Fixtures/Excel/Empleado.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="3"/>
+    <workbookView xWindow="13020" yWindow="0" windowWidth="19560" windowHeight="8340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Empleado" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -248,7 +248,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="8">
@@ -685,12 +685,35 @@
       <c r="S2" s="11">
         <v>200.1</v>
       </c>
-      <c r="T2" s="9">
-        <v>0</v>
+      <c r="T2" s="8">
+        <v>1</v>
       </c>
       <c r="U2" s="11">
         <v>209.04</v>
       </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -702,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,6 +782,13 @@
       <c r="F2" s="10">
         <v>0.04</v>
       </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E9" s="7"/>
@@ -841,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>